<commit_message>
fix pie chart opset 20
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
@@ -853,7 +853,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::60_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::25825_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::179): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::25944): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::269): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26034): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::271): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26036): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::317): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26082): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::319): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26084): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::337): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26102): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::339): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26104): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::458): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::26223): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::495): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::26260): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::966): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::26731): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::971): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::26736): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix microsoft node link
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
@@ -853,7 +853,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::29196_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::34138_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29315): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34257): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29405): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34347): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29407): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34349): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29453): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34395): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29455): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34397): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29473): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34415): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29475): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34417): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::29594): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34536): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::29631): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::34573): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::30102): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::35044): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::30107): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::35049): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add time in the opset readme
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_20/CPU/training_CPUExecutionProvider.xlsx
@@ -853,7 +853,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::34138_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::60_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34257): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::179): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34347): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::269): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34349): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::271): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34395): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::317): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34397): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::319): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34415): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::337): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34417): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::339): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::34536): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::458): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::34573): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::495): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::35044): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::966): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::35049): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::971): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>

</xml_diff>